<commit_message>
Ajustes na tela de importação de arquivo de Fornecedores
</commit_message>
<xml_diff>
--- a/Arquivos Fornecedores/oderco-teste.xlsx
+++ b/Arquivos Fornecedores/oderco-teste.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colaborador.053\Desktop\TESTE CROSSSYS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12150"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4442" uniqueCount="2652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4441" uniqueCount="2652">
   <si>
     <t>169.NN-ST252WRU.110V</t>
   </si>
@@ -7985,12 +7980,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="166" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -8082,17 +8077,17 @@
   <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
@@ -8139,12 +8134,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="4" borderId="0" xfId="12" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="6" fillId="4" borderId="0" xfId="12" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Moeda 2" xfId="2"/>
@@ -8218,7 +8213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -8253,7 +8248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -8430,7 +8425,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -8440,13 +8435,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2647"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A1719" workbookViewId="0">
+      <selection activeCell="E1740" sqref="E1740"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
@@ -34530,10 +34526,10 @@
       </c>
       <c r="C1739" s="15"/>
       <c r="D1739" s="5">
-        <v>0</v>
-      </c>
-      <c r="E1739" s="21" t="s">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E1739" s="21">
+        <v>10</v>
       </c>
     </row>
     <row r="1740" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>